<commit_message>
added general schematic for generator + made changes in expenses
</commit_message>
<xml_diff>
--- a/general objective.xlsx
+++ b/general objective.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368B8633-E7CD-4B66-BD0D-551A49349BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12528D6-0541-4D4A-B9E3-42719D4D8062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
   </bookViews>
   <sheets>
-    <sheet name="pretext" sheetId="1" r:id="rId1"/>
-    <sheet name="Materials" sheetId="3" r:id="rId2"/>
-    <sheet name="magnet selection" sheetId="2" r:id="rId3"/>
+    <sheet name="README" sheetId="1" r:id="rId1"/>
+    <sheet name="DOCUMENTS RELATED INFO" sheetId="5" r:id="rId2"/>
+    <sheet name="Expenses" sheetId="4" r:id="rId3"/>
+    <sheet name="Materials" sheetId="3" r:id="rId4"/>
+    <sheet name="Materials - Magnet Selection" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="165">
   <si>
     <t>https://youtu.be/yiD5nCfmbV0</t>
   </si>
@@ -50,9 +52,6 @@
     <t>https://hobbyking.com/en_us/blog/reading-and-understanding-lipo-batteries/?___store=en_us</t>
   </si>
   <si>
-    <t>// ndi na naten need bumili pa, meron na ako battery dito sa bahay</t>
-  </si>
-  <si>
     <t>how to know wtf is this motor's current speed</t>
   </si>
   <si>
@@ -96,9 +95,6 @@
   </si>
   <si>
     <t>microcontroller (esp32)</t>
-  </si>
-  <si>
-    <t>battery (meron na ako dito bahay)</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=uOQk8SJso6Q</t>
@@ -401,9 +397,6 @@
     <t>battery</t>
   </si>
   <si>
-    <t>2s LiPo with at least 1.5 Ah</t>
-  </si>
-  <si>
     <t>https://shopee.ph/608-608Z-608ZZ-608RS-608-2RS-Bearing-i.27267468.13275078714</t>
   </si>
   <si>
@@ -414,6 +407,147 @@
   </si>
   <si>
     <t>https://youtu.be/YYQayMrK4Fo?list=PLX-JqQpYfm1XB372KrjxN2yxgd2iYslIc</t>
+  </si>
+  <si>
+    <t>item name</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price </t>
+  </si>
+  <si>
+    <t>unique item</t>
+  </si>
+  <si>
+    <t>candidate 1 magnet</t>
+  </si>
+  <si>
+    <t>candidate 2 magnet</t>
+  </si>
+  <si>
+    <t>0.1mm 50m</t>
+  </si>
+  <si>
+    <t>potentiometer</t>
+  </si>
+  <si>
+    <t>total pesos with shipping (+40 from china)</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>coil winding</t>
+  </si>
+  <si>
+    <t>https://www.globalspec.com/pfdetail/motors/motor-winding-calculations</t>
+  </si>
+  <si>
+    <t>ano masasabi for this</t>
+  </si>
+  <si>
+    <t>hall effect sensor</t>
+  </si>
+  <si>
+    <t>https://electronoobs.com/eng_arduino_tut82.php</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AH49E.pdf</t>
+  </si>
+  <si>
+    <t>guide how to use</t>
+  </si>
+  <si>
+    <t>bldc diy</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wB1mUEClcNk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fast af </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Wqr1b4mWDsE</t>
+  </si>
+  <si>
+    <t>battery holder (for 3 batteries in series)</t>
+  </si>
+  <si>
+    <t>3 batteries</t>
+  </si>
+  <si>
+    <t>18650 3Ah</t>
+  </si>
+  <si>
+    <t>aligator clips</t>
+  </si>
+  <si>
+    <t>49E</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>https://www.quora.com/Increasing-the-number-of-coil-windings-on-an-electric-motor-does-not-always-increase-the-HP-of-the-motor-Therefore-what-does-the-number-of-windings-and-power-curve-look-like-for-an-electric-motor</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>supporting details</t>
+  </si>
+  <si>
+    <t>jakob scherer = supporting argument</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>3s Li-ion/LiPo with at least 1.5 Ah</t>
+  </si>
+  <si>
+    <t>https://shopee.ph/PKCell-3.7V-Lithium-ion-NMC-18650-21700-Battery-for-Solar-Electric-Scooter-Mini-Fan-Power-Bank-i.18252381.1670629656</t>
+  </si>
+  <si>
+    <t>https://shopee.ph/60m-10m-of-Magnet-Wire-Enameled-Copper-Wire-Winding-For-Making-Electromagnet-Motor-0.1mm-0.2mm-0.3mm-0.4mm-0.5mm-0.6mm-0.7mm-0.8mm-0.9mm-i.866205405.18246963879</t>
+  </si>
+  <si>
+    <t>https://shopee.ph/10pcs-Alligator-Clips-Electrical-DIY-Test-Leads-Alligator-Double-ended-Crocodile-Clips-Test-i.8710520.18989319838</t>
+  </si>
+  <si>
+    <t>https://shopee.ph/10pcs-A3144-OH3144-OH137-49E-Hall-Effect-Sensor-Brushless-Electric-Motor-TO-92UA-A3144EUA-i.487295469.10441228144</t>
+  </si>
+  <si>
+    <t>https://shopee.ph/Series-Battery-Holder-18650-with-Wire-1-Cell-2-Cell-3-Cell-1S-2S-3S-Single-Double-Triple-i.18252381.453473950</t>
+  </si>
+  <si>
+    <t>https://shopee.ph/5-PCS-B10k-Rotary-Knob-type-10k-Ohm-Precision-Potentiometer-i.18252381.13228237269</t>
+  </si>
+  <si>
+    <t>bk10 metallic</t>
+  </si>
+  <si>
+    <t>fidget spinner</t>
+  </si>
+  <si>
+    <t>wtf</t>
+  </si>
+  <si>
+    <t>wtf 5 hands</t>
+  </si>
+  <si>
+    <t>\- hilasque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">will be updated further </t>
+  </si>
+  <si>
+    <t>ples read these mdfking references</t>
+  </si>
+  <si>
+    <t>then consult these for details</t>
   </si>
 </sst>
 </file>
@@ -470,7 +604,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,8 +647,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -734,12 +874,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -809,60 +960,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1179,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E93D857-947A-4A64-B2A3-955470D1FDE7}">
-  <dimension ref="B3:K42"/>
+  <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,232 +1357,237 @@
     <col min="4" max="4" width="34.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+    </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="46" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="46"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="44"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+    </row>
+    <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="46"/>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="48"/>
+    </row>
+    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="46"/>
+      <c r="D7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="52"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C9" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C10" s="45"/>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="48"/>
-    </row>
-    <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="44"/>
-      <c r="D6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="46"/>
-    </row>
-    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="44"/>
-      <c r="D7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="43"/>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="37" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C13" s="41"/>
-      <c r="E13" t="s">
-        <v>7</v>
+      <c r="C13" s="43"/>
+      <c r="E13" s="37" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="37" t="s">
         <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="36.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="2:11" ht="31.2" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="59" t="s">
-        <v>119</v>
+      <c r="B19" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>116</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="46"/>
+        <v>29</v>
+      </c>
+      <c r="E19" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="48"/>
     </row>
     <row r="25" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B25" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="43" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C27" s="41" t="s">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="43"/>
+      <c r="E28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="43"/>
+      <c r="E29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="41"/>
-      <c r="E28" t="s">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="43"/>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="43"/>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="J31" s="37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="43"/>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C33" s="43"/>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C34" s="43"/>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="J34" s="37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="41"/>
-      <c r="E29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C30" s="41"/>
-      <c r="E30" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C31" s="41"/>
-      <c r="E31" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C32" s="41"/>
-      <c r="E32" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C33" s="41"/>
-      <c r="E33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C34" s="41"/>
-      <c r="E34" t="s">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C35" s="43"/>
+      <c r="E35" t="s">
         <v>14</v>
       </c>
-      <c r="J34" s="37" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C35" s="41"/>
-      <c r="E35" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C36" s="41"/>
+      <c r="C36" s="43"/>
       <c r="E36" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C38" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C41" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C42" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1437,153 +1606,654 @@
     <hyperlink ref="E7" r:id="rId1" xr:uid="{3E48C770-EAE1-452F-8FB4-BC563B4E1D3F}"/>
     <hyperlink ref="J34" r:id="rId2" xr:uid="{575FCEDD-73DC-4FC1-88F4-C09ADC5D2426}"/>
     <hyperlink ref="J31" r:id="rId3" xr:uid="{E63AAF86-C271-47E1-87CC-DBFE774B7269}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{9F43ED7E-D341-4A0D-8ABD-1C022AB180B5}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{1B54A2F6-4125-4CDF-948D-25B46E851B9A}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{00B071E8-A202-456F-B0B7-F8906BD1E6D5}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{74A1CDCC-2F3E-4F85-8BA6-8144A28A2D61}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{57FC4031-A295-4C34-B5BB-76416AD8BDD7}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{75D8BA65-7AD0-4719-9660-E354A16F3C2E}"/>
+    <hyperlink ref="E15" r:id="rId10" xr:uid="{17FD8866-3235-435E-9006-DAED38E08963}"/>
+    <hyperlink ref="E19" r:id="rId11" xr:uid="{587957E1-40B2-4A94-8B1E-7BD7069343CE}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{E72DBF15-9875-412D-9D8C-7A66F619673A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23162244-2321-4040-8FBF-AD0CA3B741BA}">
-  <dimension ref="B3:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F323EC37-910C-43FB-ABC5-682BD73B1403}">
+  <dimension ref="A4:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>1</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B11" s="61"/>
+      <c r="C11" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="B13" s="61"/>
+      <c r="C13" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="B15" s="61"/>
+      <c r="C15" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="63"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="63"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="63"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="63"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="63"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="63"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="63"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="63"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="63"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{9901E4ED-5E8F-48CC-89B9-3F506624C58D}"/>
+    <hyperlink ref="C10" r:id="rId2" xr:uid="{1C90D308-8BDF-4324-8358-B3895635D1E7}"/>
+    <hyperlink ref="C12" r:id="rId3" xr:uid="{7FF92000-990C-440C-AD88-A184181C85FB}"/>
+    <hyperlink ref="C13" r:id="rId4" xr:uid="{82838CCE-44FE-4D70-90B2-AD6A77EF51ED}"/>
+    <hyperlink ref="C14" r:id="rId5" xr:uid="{40EDC363-0C8E-4B5C-A177-F4C5254B280E}"/>
+    <hyperlink ref="C15" r:id="rId6" xr:uid="{3B702C57-C53E-470D-952B-7B51DCF022BE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41353588-76EC-44BD-8AE0-3352EC381993}">
+  <dimension ref="A2:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="31.77734375" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="62" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>239</v>
+      </c>
+      <c r="E3" s="2">
+        <v>269</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>27</v>
+      </c>
+      <c r="E4" s="2">
+        <v>148</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>48</v>
+      </c>
+      <c r="E5" s="2">
+        <v>88</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>468</v>
+      </c>
+      <c r="E6" s="2">
+        <f>468+40</f>
+        <v>508</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>70</v>
+      </c>
+      <c r="E7" s="2">
+        <v>108</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" s="37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>166</v>
+      </c>
+      <c r="E8" s="44">
+        <v>272</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>68</v>
+      </c>
+      <c r="E9" s="45"/>
+      <c r="F9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="62">
+        <v>8</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="62">
+        <v>1</v>
+      </c>
+      <c r="D10" s="62">
+        <v>64</v>
+      </c>
+      <c r="E10" s="62">
+        <v>102</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="62">
+        <v>9</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="62">
+        <v>1</v>
+      </c>
+      <c r="D11" s="62">
+        <v>66</v>
+      </c>
+      <c r="E11" s="62">
+        <v>106</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="64">
+        <v>10</v>
+      </c>
+      <c r="B12" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="64">
+        <v>1</v>
+      </c>
+      <c r="D12" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="E12" s="65" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" s="65" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14">
+        <f>SUM(E3:E13)</f>
+        <v>1601</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E8:E9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{D2FC49C8-05CC-47ED-BCF6-9D96E9942701}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{35AFD705-ACBC-4A07-A26B-A8A59E6F3AAC}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{F4194F14-90F1-420A-BC35-0368152BA4D0}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{C86BDC45-B621-4FE8-A88D-B37E08B978E9}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{D3F08C4D-B68B-444B-A2A8-52191DB58905}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{2EAE62F6-EBB0-4478-9BAE-90BD73E253D2}"/>
+    <hyperlink ref="G9" r:id="rId7" xr:uid="{151D7C36-72F1-4355-967B-26BCF2CC295D}"/>
+    <hyperlink ref="G10" r:id="rId8" xr:uid="{934278AD-0999-4496-8F46-AFBCAE2410AA}"/>
+    <hyperlink ref="G11" r:id="rId9" xr:uid="{984CBBDC-41E6-4C5E-9C39-2782D43B70E3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23162244-2321-4040-8FBF-AD0CA3B741BA}">
+  <dimension ref="B2:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.44140625" customWidth="1"/>
     <col min="5" max="5" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+    </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="E3" s="38" t="s">
         <v>97</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -1592,44 +2262,44 @@
     </row>
     <row r="13" spans="2:5" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E14" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1643,12 +2313,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617951F-4090-4031-B4D9-7E54778FB332}">
   <dimension ref="E1:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1663,57 +2333,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="E1" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
+      <c r="E1" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
     </row>
     <row r="2" spans="5:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="J2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="M2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="P2" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="5:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1747,16 +2417,16 @@
         <v>239</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="5:16" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1790,16 +2460,16 @@
         <v>216</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="5:16" x14ac:dyDescent="0.3">
@@ -1833,16 +2503,16 @@
         <v>220</v>
       </c>
       <c r="M5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="P5" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="5:16" x14ac:dyDescent="0.3">
@@ -1876,16 +2546,16 @@
         <v>110</v>
       </c>
       <c r="M6" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="P6" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="5:16" x14ac:dyDescent="0.3">
@@ -1919,16 +2589,16 @@
         <v>360</v>
       </c>
       <c r="M7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="P7" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="5:16" x14ac:dyDescent="0.3">
@@ -1962,33 +2632,33 @@
         <v>552</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="5:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="5:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="F11" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="53"/>
-      <c r="N11" s="53"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="54"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="56"/>
     </row>
     <row r="12" spans="5:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E12" s="13"/>
@@ -1997,27 +2667,27 @@
         <v>6</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L12" s="16"/>
       <c r="M12" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P12" s="19"/>
     </row>
     <row r="13" spans="5:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L13" s="16"/>
       <c r="M13" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="O13" s="22" t="s">
         <v>66</v>
-      </c>
-      <c r="N13" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="O13" s="22" t="s">
-        <v>68</v>
       </c>
       <c r="P13" s="23">
         <v>64</v>
@@ -2025,20 +2695,20 @@
     </row>
     <row r="14" spans="5:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L14" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M14" s="25">
         <v>8</v>
       </c>
       <c r="N14" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O14" s="22"/>
       <c r="P14" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="5:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2047,46 +2717,46 @@
         <v>300</v>
       </c>
       <c r="G15" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="L16" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="H15" s="27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="L16" s="55" t="s">
-        <v>75</v>
-      </c>
-      <c r="M16" s="56"/>
+      <c r="M16" s="58"/>
     </row>
     <row r="17" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="L17" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="5:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="L18" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="M18" s="57" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="M18" s="59" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.3">
       <c r="L19" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="M19" s="57"/>
+        <v>78</v>
+      </c>
+      <c r="M19" s="59"/>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2095,10 +2765,10 @@
         <v>212.05750411731105</v>
       </c>
       <c r="G21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2107,18 +2777,18 @@
         <v>70.685834705770347</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2127,19 +2797,19 @@
         <v>706.85834705770344</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="29" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G29" s="33"/>
     </row>
@@ -2149,29 +2819,29 @@
         <v>400</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="6:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F33" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G33" s="15">
         <f>20*20</f>
         <v>400</v>
       </c>
       <c r="H33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G34">
         <v>3</v>
@@ -2179,7 +2849,7 @@
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G35">
         <f>G33*G34</f>

</xml_diff>

<commit_message>
added +2 more batteries (previously 1) in EXPENSES
</commit_message>
<xml_diff>
--- a/general objective.xlsx
+++ b/general objective.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031831FF-ED71-4C79-A5CC-828010E7674A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F6572C-DFD2-498B-877B-DFD9023CCA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
   </bookViews>
@@ -547,10 +547,10 @@
     <t>wtf 5 limbs</t>
   </si>
   <si>
-    <t>total pesos with shipping</t>
-  </si>
-  <si>
     <t>REMOVED</t>
+  </si>
+  <si>
+    <t>total pesos with shipping + (38 ph, 40 ch)</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E93D857-947A-4A64-B2A3-955470D1FDE7}">
   <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -1756,13 +1756,13 @@
   <dimension ref="A2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="31.77734375" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
   </cols>
@@ -1781,7 +1781,7 @@
         <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>121</v>
@@ -1850,6 +1850,7 @@
         <v>48</v>
       </c>
       <c r="E5" s="2">
+        <f>D5+40</f>
         <v>88</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -1873,7 +1874,7 @@
         <v>468</v>
       </c>
       <c r="E6" s="2">
-        <f>468+40</f>
+        <f>D6+40</f>
         <v>508</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -1897,6 +1898,7 @@
         <v>70</v>
       </c>
       <c r="E7" s="2">
+        <f>D7+38</f>
         <v>108</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -1917,10 +1919,12 @@
         <v>1</v>
       </c>
       <c r="D8" s="2">
-        <v>166</v>
+        <f>166+169+169</f>
+        <v>504</v>
       </c>
       <c r="E8" s="46">
-        <v>272</v>
+        <f>D8+D9+38</f>
+        <v>610</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>140</v>
@@ -1964,6 +1968,7 @@
         <v>64</v>
       </c>
       <c r="E10" s="2">
+        <f>D10+38</f>
         <v>102</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -1987,6 +1992,7 @@
         <v>66</v>
       </c>
       <c r="E11" s="2">
+        <f>D11+40</f>
         <v>106</v>
       </c>
       <c r="F11" s="2" t="s">
@@ -2025,12 +2031,12 @@
       </c>
       <c r="E14">
         <f>SUM(E3:E13)</f>
-        <v>1480</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2288,7 +2294,7 @@
   <dimension ref="E1:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added a source for bldc motor fundamentals paper
</commit_message>
<xml_diff>
--- a/general objective.xlsx
+++ b/general objective.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F6572C-DFD2-498B-877B-DFD9023CCA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA24D2DB-FA50-4128-94D7-A18CFE802170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="165">
   <si>
     <t>https://youtu.be/yiD5nCfmbV0</t>
   </si>
@@ -526,15 +526,6 @@
     <t>bk10 metallic</t>
   </si>
   <si>
-    <t>fidget spinner</t>
-  </si>
-  <si>
-    <t>wtf</t>
-  </si>
-  <si>
-    <t>\- hilasque</t>
-  </si>
-  <si>
     <t xml:space="preserve">will be updated further </t>
   </si>
   <si>
@@ -544,13 +535,19 @@
     <t>then consult these for details</t>
   </si>
   <si>
-    <t>wtf 5 limbs</t>
-  </si>
-  <si>
     <t>REMOVED</t>
   </si>
   <si>
     <t>total pesos with shipping + (38 ph, 40 ch)</t>
+  </si>
+  <si>
+    <t>https://www.monolithicpower.com/media/document/Brushless_DC_Motor_Fundamentals.pdf</t>
+  </si>
+  <si>
+    <t>all r good resource</t>
+  </si>
+  <si>
+    <t>bldc fundamentals</t>
   </si>
 </sst>
 </file>
@@ -607,7 +604,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -650,12 +647,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -893,7 +884,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -967,8 +958,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1029,6 +1018,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1360,7 +1352,7 @@
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1368,61 +1360,61 @@
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="46" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="51"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="49"/>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="48"/>
+      <c r="C5" s="46"/>
       <c r="D5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="54"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="52"/>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="48"/>
+      <c r="C6" s="46"/>
       <c r="D6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="51"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="49"/>
     </row>
     <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="48"/>
+      <c r="C7" s="46"/>
       <c r="D7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="E7" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="55"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="53"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="44" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
@@ -1433,7 +1425,7 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C10" s="47"/>
+      <c r="C10" s="45"/>
       <c r="D10" t="s">
         <v>25</v>
       </c>
@@ -1442,7 +1434,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="43" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="37" t="s">
@@ -1450,7 +1442,7 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C13" s="45"/>
+      <c r="C13" s="43"/>
       <c r="E13" s="37" t="s">
         <v>137</v>
       </c>
@@ -1474,15 +1466,15 @@
       <c r="D19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="49" t="s">
+      <c r="E19" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="51"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="49"/>
     </row>
     <row r="25" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B25" s="6" t="s">
@@ -1490,30 +1482,30 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="43" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="45"/>
+      <c r="C28" s="43"/>
       <c r="E28" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="45"/>
+      <c r="C29" s="43"/>
       <c r="E29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C30" s="45"/>
+      <c r="C30" s="43"/>
       <c r="E30" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C31" s="45"/>
+      <c r="C31" s="43"/>
       <c r="E31" t="s">
         <v>20</v>
       </c>
@@ -1522,19 +1514,19 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C32" s="45"/>
+      <c r="C32" s="43"/>
       <c r="E32" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C33" s="45"/>
+      <c r="C33" s="43"/>
       <c r="E33" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C34" s="45"/>
+      <c r="C34" s="43"/>
       <c r="E34" t="s">
         <v>13</v>
       </c>
@@ -1543,13 +1535,13 @@
       </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C35" s="45"/>
+      <c r="C35" s="43"/>
       <c r="E35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C36" s="45"/>
+      <c r="C36" s="43"/>
       <c r="E36" t="s">
         <v>35</v>
       </c>
@@ -1623,10 +1615,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F323EC37-910C-43FB-ABC5-682BD73B1403}">
-  <dimension ref="A4:D15"/>
+  <dimension ref="A4:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1638,7 +1630,7 @@
   <sheetData>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1659,7 +1651,7 @@
       <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="54" t="s">
         <v>127</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -1673,7 +1665,7 @@
       <c r="A11" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B11" s="57"/>
+      <c r="B11" s="55"/>
       <c r="C11" s="12" t="s">
         <v>144</v>
       </c>
@@ -1685,7 +1677,7 @@
       <c r="A12" s="2">
         <v>2</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="54" t="s">
         <v>130</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -1699,7 +1691,7 @@
       <c r="A13" s="2">
         <v>2.1</v>
       </c>
-      <c r="B13" s="57"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="12" t="s">
         <v>131</v>
       </c>
@@ -1711,7 +1703,7 @@
       <c r="A14" s="2">
         <v>3</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="54" t="s">
         <v>134</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -1725,12 +1717,26 @@
       <c r="A15" s="2">
         <v>3.1</v>
       </c>
-      <c r="B15" s="57"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="12" t="s">
         <v>137</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="65">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="65" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1746,6 +1752,7 @@
     <hyperlink ref="C13" r:id="rId4" xr:uid="{82838CCE-44FE-4D70-90B2-AD6A77EF51ED}"/>
     <hyperlink ref="C14" r:id="rId5" xr:uid="{40EDC363-0C8E-4B5C-A177-F4C5254B280E}"/>
     <hyperlink ref="C15" r:id="rId6" xr:uid="{3B702C57-C53E-470D-952B-7B51DCF022BE}"/>
+    <hyperlink ref="C16" r:id="rId7" xr:uid="{02E26761-472F-4897-B5F6-00BC99B6EFE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1755,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41353588-76EC-44BD-8AE0-3352EC381993}">
   <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1781,7 +1788,7 @@
         <v>120</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>121</v>
@@ -1922,7 +1929,7 @@
         <f>166+169+169</f>
         <v>504</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="44">
         <f>D8+D9+38</f>
         <v>610</v>
       </c>
@@ -1946,7 +1953,7 @@
       <c r="D9" s="2">
         <v>68</v>
       </c>
-      <c r="E9" s="47"/>
+      <c r="E9" s="45"/>
       <c r="F9" s="2" t="s">
         <v>139</v>
       </c>
@@ -2003,40 +2010,26 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="43">
-        <v>10</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="43">
-        <v>1</v>
-      </c>
-      <c r="D12" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="G12" s="44" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D14" t="s">
+      <c r="A12" s="63"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="64"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
         <v>143</v>
       </c>
-      <c r="E14">
+      <c r="E19">
         <f>SUM(E3:E13)</f>
         <v>1818</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -2101,7 +2094,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
@@ -2310,20 +2303,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
     </row>
     <row r="2" spans="5:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="2" t="s">
@@ -2629,13 +2622,13 @@
       <c r="F11" t="s">
         <v>59</v>
       </c>
-      <c r="L11" s="59" t="s">
+      <c r="L11" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="61"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="59"/>
     </row>
     <row r="12" spans="5:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E12" s="13"/>
@@ -2701,10 +2694,10 @@
       </c>
     </row>
     <row r="16" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="L16" s="62" t="s">
+      <c r="L16" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="M16" s="63"/>
+      <c r="M16" s="61"/>
     </row>
     <row r="17" spans="5:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="L17" s="28" t="s">
@@ -2718,7 +2711,7 @@
       <c r="L18" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="M18" s="64" t="s">
+      <c r="M18" s="62" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2726,7 +2719,7 @@
       <c r="L19" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="M19" s="64"/>
+      <c r="M19" s="62"/>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.3">
       <c r="E20" t="s">

</xml_diff>

<commit_message>
objective revision + added designs
</commit_message>
<xml_diff>
--- a/general objective.xlsx
+++ b/general objective.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EACC96-3086-4316-B07E-BF352538784A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980A28E1-3A52-4CD6-B9A2-D6187AE3C6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
-    <sheet name="DOCUMENTS RELATED INFO" sheetId="5" r:id="rId2"/>
-    <sheet name="Expenses" sheetId="4" r:id="rId3"/>
-    <sheet name="Materials" sheetId="3" r:id="rId4"/>
-    <sheet name="Materials - Magnet Selection" sheetId="2" r:id="rId5"/>
+    <sheet name="General guidelines" sheetId="6" r:id="rId2"/>
+    <sheet name="DOCUMENTS RELATED INFO" sheetId="5" r:id="rId3"/>
+    <sheet name="Expenses" sheetId="4" r:id="rId4"/>
+    <sheet name="Materials" sheetId="3" r:id="rId5"/>
+    <sheet name="Materials - Magnet Selection" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="172">
   <si>
     <t>https://youtu.be/yiD5nCfmbV0</t>
   </si>
@@ -554,6 +555,21 @@
   </si>
   <si>
     <t>https://shopee.ph/Logic-Level-Converter-%E2%80%93-Bi-Directional-i.18252381.255177311</t>
+  </si>
+  <si>
+    <t>gawin muna natin ung paper (intro-objectives and limitations, and rrl)</t>
+  </si>
+  <si>
+    <t>tapos base dun sa mga naresearch nating theory in relation sa electromagnets at ung bldc motors, gawa na tayo ng design (which is ung methodology)</t>
+  </si>
+  <si>
+    <t>meron na tayong placeholder design (temporary; nadecide kahapon sa meeting), pero magkaroroon ng minor changes dun after ng #1 step</t>
+  </si>
+  <si>
+    <t>ang gist ng design:</t>
+  </si>
+  <si>
+    <t>motor</t>
   </si>
 </sst>
 </file>
@@ -1042,6 +1058,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>54430</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>174172</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>428476</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>83173</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D11779-8DB0-CD14-B560-D4658EDDA51B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13465630" y="9797143"/>
+          <a:ext cx="7689246" cy="5090601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>108858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>595146</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>55962</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8058E371-FCB3-8A95-F36E-9291882BB8EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3124201" y="9916887"/>
+          <a:ext cx="9053345" cy="5128704"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>359229</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>130629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>54878</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>6874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14C6E59B-4F4B-50DB-21BE-FDA74C8A7753}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="968829" y="2166258"/>
+          <a:ext cx="5182049" cy="3947502"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>16454</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>416579</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1593</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{879CE478-EB7F-1F19-80B9-59A42C2A2835}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6749143" y="1867025"/>
+          <a:ext cx="7078636" cy="4796625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1343,7 +1540,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E93D857-947A-4A64-B2A3-955470D1FDE7}">
   <dimension ref="B2:K42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
@@ -1619,6 +1816,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18F05EE-8DBB-4778-986E-BA0587C5A8CE}">
+  <dimension ref="B4:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB14" sqref="AB14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F323EC37-910C-43FB-ABC5-682BD73B1403}">
   <dimension ref="A4:D16"/>
   <sheetViews>
@@ -1763,11 +2007,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41353588-76EC-44BD-8AE0-3352EC381993}">
   <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -2097,7 +2341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23162244-2321-4040-8FBF-AD0CA3B741BA}">
   <dimension ref="B2:E15"/>
   <sheetViews>
@@ -2303,7 +2547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617951F-4090-4031-B4D9-7E54778FB332}">
   <dimension ref="E1:P35"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated readme for the recent objective (creating a bldc motor)
</commit_message>
<xml_diff>
--- a/general objective.xlsx
+++ b/general objective.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDD6381-06BA-487C-AB5D-83B3E65E1016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427447A2-645A-4A56-838D-BAF6D00E9A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
   </bookViews>
   <sheets>
     <sheet name="General guidelines" sheetId="6" r:id="rId1"/>
@@ -1157,33 +1157,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1194,18 +1206,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1856,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18F05EE-8DBB-4778-986E-BA0587C5A8CE}">
   <dimension ref="B4:AA159"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P91" sqref="P91"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1909,7 +1909,7 @@
       </c>
     </row>
     <row r="50" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M50" s="52" t="s">
+      <c r="M50" s="51" t="s">
         <v>169</v>
       </c>
       <c r="N50" s="2" t="s">
@@ -1920,19 +1920,19 @@
       </c>
     </row>
     <row r="51" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M51" s="52"/>
+      <c r="M51" s="51"/>
       <c r="N51" s="2" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="52" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M52" s="52"/>
+      <c r="M52" s="51"/>
       <c r="N52" s="2" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="53" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M53" s="52" t="s">
+      <c r="M53" s="51" t="s">
         <v>173</v>
       </c>
       <c r="N53" s="2" t="s">
@@ -1940,13 +1940,13 @@
       </c>
     </row>
     <row r="54" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M54" s="52"/>
+      <c r="M54" s="51"/>
       <c r="N54" s="2" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="55" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M55" s="52" t="s">
+      <c r="M55" s="51" t="s">
         <v>205</v>
       </c>
       <c r="N55" s="2" t="s">
@@ -1954,19 +1954,19 @@
       </c>
     </row>
     <row r="56" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M56" s="52"/>
+      <c r="M56" s="51"/>
       <c r="N56" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="57" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M57" s="52"/>
+      <c r="M57" s="51"/>
       <c r="N57" s="2" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="58" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M58" s="52"/>
+      <c r="M58" s="51"/>
       <c r="N58" s="2" t="s">
         <v>12</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="J125" s="47" t="s">
         <v>194</v>
       </c>
-      <c r="K125" s="53" t="s">
+      <c r="K125" s="52" t="s">
         <v>196</v>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       <c r="J126" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="K126" s="53"/>
+      <c r="K126" s="52"/>
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J127" s="29" t="s">
@@ -2044,7 +2044,7 @@
       </c>
     </row>
     <row r="133" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J133" s="50"/>
+      <c r="J133" s="49"/>
       <c r="K133" s="46" t="s">
         <v>196</v>
       </c>
@@ -2053,7 +2053,7 @@
       </c>
     </row>
     <row r="134" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J134" s="49"/>
+      <c r="J134" s="50"/>
       <c r="K134" s="46" t="s">
         <v>168</v>
       </c>
@@ -2070,7 +2070,7 @@
       </c>
     </row>
     <row r="137" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J137" s="49"/>
+      <c r="J137" s="50"/>
       <c r="K137" s="46" t="s">
         <v>196</v>
       </c>
@@ -2090,7 +2090,7 @@
       </c>
     </row>
     <row r="141" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J141" s="49"/>
+      <c r="J141" s="50"/>
       <c r="K141" s="2" t="s">
         <v>168</v>
       </c>
@@ -2110,7 +2110,7 @@
       </c>
     </row>
     <row r="144" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J144" s="49"/>
+      <c r="J144" s="50"/>
       <c r="K144" s="2" t="s">
         <v>196</v>
       </c>
@@ -2136,13 +2136,13 @@
       </c>
     </row>
     <row r="149" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="J149" s="50"/>
+      <c r="J149" s="49"/>
       <c r="K149" s="2" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="150" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="J150" s="49"/>
+      <c r="J150" s="50"/>
       <c r="K150" s="2" t="s">
         <v>196</v>
       </c>
@@ -2157,7 +2157,7 @@
       <c r="I153" t="s">
         <v>191</v>
       </c>
-      <c r="J153" s="51" t="s">
+      <c r="J153" s="53" t="s">
         <v>200</v>
       </c>
       <c r="K153" s="2" t="s">
@@ -2165,13 +2165,13 @@
       </c>
     </row>
     <row r="154" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="J154" s="51"/>
+      <c r="J154" s="53"/>
       <c r="K154" s="2" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="155" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="J155" s="51"/>
+      <c r="J155" s="53"/>
       <c r="K155" s="2" t="s">
         <v>196</v>
       </c>
@@ -2183,16 +2183,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J140:J141"/>
+    <mergeCell ref="J143:J144"/>
+    <mergeCell ref="J148:J150"/>
+    <mergeCell ref="J153:J155"/>
+    <mergeCell ref="J136:J137"/>
     <mergeCell ref="J132:J134"/>
     <mergeCell ref="M50:M52"/>
     <mergeCell ref="M55:M58"/>
     <mergeCell ref="M53:M54"/>
     <mergeCell ref="K125:K126"/>
-    <mergeCell ref="J140:J141"/>
-    <mergeCell ref="J143:J144"/>
-    <mergeCell ref="J148:J150"/>
-    <mergeCell ref="J153:J155"/>
-    <mergeCell ref="J136:J137"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2203,7 +2203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1EE407-BF25-41AB-851C-5DD43D85D019}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2409,7 +2409,7 @@
       <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="59" t="s">
         <v>127</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -2423,7 +2423,7 @@
       <c r="A11" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B11" s="65"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="12" t="s">
         <v>144</v>
       </c>
@@ -2435,7 +2435,7 @@
       <c r="A12" s="2">
         <v>2</v>
       </c>
-      <c r="B12" s="64" t="s">
+      <c r="B12" s="59" t="s">
         <v>130</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2449,7 +2449,7 @@
       <c r="A13" s="2">
         <v>2.1</v>
       </c>
-      <c r="B13" s="65"/>
+      <c r="B13" s="60"/>
       <c r="C13" s="12" t="s">
         <v>131</v>
       </c>
@@ -2461,7 +2461,7 @@
       <c r="A14" s="2">
         <v>3</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="59" t="s">
         <v>134</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -2475,7 +2475,7 @@
       <c r="A15" s="2">
         <v>3.1</v>
       </c>
-      <c r="B15" s="65"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="12" t="s">
         <v>137</v>
       </c>
@@ -2507,61 +2507,61 @@
       <c r="B29" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="61" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="55" t="s">
+      <c r="E29" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="58"/>
     </row>
     <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C30" s="54"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="58" t="s">
+      <c r="E30" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="60"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="64"/>
     </row>
     <row r="31" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="54"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="58"/>
     </row>
     <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="54"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="55"/>
-      <c r="I32" s="61"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="65"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C34" s="62" t="s">
+      <c r="C34" s="54" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
@@ -2572,7 +2572,7 @@
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C35" s="63"/>
+      <c r="C35" s="55"/>
       <c r="D35" t="s">
         <v>25</v>
       </c>
@@ -2581,7 +2581,7 @@
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C37" s="52" t="s">
+      <c r="C37" s="51" t="s">
         <v>5</v>
       </c>
       <c r="E37" s="37" t="s">
@@ -2589,7 +2589,7 @@
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C38" s="52"/>
+      <c r="C38" s="51"/>
       <c r="E38" s="37" t="s">
         <v>137</v>
       </c>
@@ -2613,15 +2613,15 @@
       <c r="D44" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E44" s="55" t="s">
+      <c r="E44" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="56"/>
-      <c r="J44" s="56"/>
-      <c r="K44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="57"/>
+      <c r="J44" s="57"/>
+      <c r="K44" s="58"/>
     </row>
     <row r="50" spans="2:10" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B50" s="6" t="s">
@@ -2629,30 +2629,30 @@
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C52" s="52" t="s">
+      <c r="C52" s="51" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C53" s="52"/>
+      <c r="C53" s="51"/>
       <c r="E53" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C54" s="52"/>
+      <c r="C54" s="51"/>
       <c r="E54" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C55" s="52"/>
+      <c r="C55" s="51"/>
       <c r="E55" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C56" s="52"/>
+      <c r="C56" s="51"/>
       <c r="E56" t="s">
         <v>20</v>
       </c>
@@ -2661,19 +2661,19 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C57" s="52"/>
+      <c r="C57" s="51"/>
       <c r="E57" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C58" s="52"/>
+      <c r="C58" s="51"/>
       <c r="E58" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C59" s="52"/>
+      <c r="C59" s="51"/>
       <c r="E59" t="s">
         <v>13</v>
       </c>
@@ -2682,13 +2682,13 @@
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C60" s="52"/>
+      <c r="C60" s="51"/>
       <c r="E60" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C61" s="52"/>
+      <c r="C61" s="51"/>
       <c r="E61" t="s">
         <v>35</v>
       </c>
@@ -2941,7 +2941,7 @@
         <f>166+169+169</f>
         <v>504</v>
       </c>
-      <c r="E8" s="62">
+      <c r="E8" s="54">
         <f>D8+D9+38</f>
         <v>610</v>
       </c>
@@ -2965,7 +2965,7 @@
       <c r="D9" s="2">
         <v>68</v>
       </c>
-      <c r="E9" s="63"/>
+      <c r="E9" s="55"/>
       <c r="F9" s="2" t="s">
         <v>139</v>
       </c>
@@ -3331,20 +3331,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
     </row>
     <row r="2" spans="5:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="2" t="s">

</xml_diff>

<commit_message>
working servo lib - just go broombroom and c the broombroom
</commit_message>
<xml_diff>
--- a/general objective.xlsx
+++ b/general objective.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1791878-5762-42B1-BDAB-F0F7D88F09A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D4331F-FE3E-4DA5-82B1-FDEE283041E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{43969D58-BB31-47A6-900F-0CFEDA7ECAD4}"/>
   </bookViews>
   <sheets>
     <sheet name="General guidelines" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="224">
   <si>
     <t>https://youtu.be/yiD5nCfmbV0</t>
   </si>
@@ -551,12 +551,6 @@
     <t>bldc fundamentals</t>
   </si>
   <si>
-    <t>bi directional level shift</t>
-  </si>
-  <si>
-    <t>https://shopee.ph/Logic-Level-Converter-%E2%80%93-Bi-Directional-i.18252381.255177311</t>
-  </si>
-  <si>
     <t>ang gist ng design:</t>
   </si>
   <si>
@@ -726,6 +720,12 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>bec output</t>
+  </si>
+  <si>
+    <t>Li-ion battery</t>
   </si>
 </sst>
 </file>
@@ -1154,20 +1154,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1853,7 +1853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18F05EE-8DBB-4778-986E-BA0587C5A8CE}">
   <dimension ref="B4:AA155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B135" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M141" sqref="M141"/>
     </sheetView>
   </sheetViews>
@@ -1866,152 +1866,152 @@
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="M10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="13:27" x14ac:dyDescent="0.3">
       <c r="M49" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M50" s="52" t="s">
-        <v>169</v>
+      <c r="M50" s="51" t="s">
+        <v>167</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>98</v>
       </c>
       <c r="AA50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M51" s="52"/>
+      <c r="M51" s="51"/>
       <c r="N51" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="52" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M52" s="52"/>
+      <c r="M52" s="51"/>
       <c r="N52" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="53" spans="13:27" x14ac:dyDescent="0.3">
+      <c r="M53" s="51" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="53" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M53" s="52" t="s">
-        <v>173</v>
       </c>
       <c r="N53" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="54" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M54" s="52"/>
+      <c r="M54" s="51"/>
       <c r="N54" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="55" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M55" s="52" t="s">
-        <v>204</v>
+      <c r="M55" s="51" t="s">
+        <v>202</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M56" s="52"/>
+      <c r="M56" s="51"/>
       <c r="N56" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="57" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M57" s="52"/>
+      <c r="M57" s="51"/>
       <c r="N57" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="13:27" x14ac:dyDescent="0.3">
-      <c r="M58" s="52"/>
+      <c r="M58" s="51"/>
       <c r="N58" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="79" spans="4:17" x14ac:dyDescent="0.3">
       <c r="D79" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="Q79" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="116" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C116" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="117" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C117" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="125" spans="2:11" x14ac:dyDescent="0.3">
       <c r="I125" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J125" s="47" t="s">
+        <v>192</v>
+      </c>
+      <c r="K125" s="52" t="s">
         <v>194</v>
-      </c>
-      <c r="K125" s="53" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="126" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J126" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="K126" s="53"/>
+        <v>193</v>
+      </c>
+      <c r="K126" s="52"/>
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J127" s="29" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K127" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="128" spans="2:11" x14ac:dyDescent="0.3">
@@ -2028,48 +2028,48 @@
     </row>
     <row r="132" spans="9:18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I132" t="s">
+        <v>195</v>
+      </c>
+      <c r="J132" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="J132" s="48" t="s">
+      <c r="K132" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="R132" t="s">
         <v>199</v>
       </c>
-      <c r="K132" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="R132" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="133" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J133" s="50"/>
+      <c r="J133" s="49"/>
       <c r="K133" s="46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="R133" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J134" s="49"/>
+      <c r="J134" s="50"/>
       <c r="K134" s="46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="136" spans="9:18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I136" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J136" s="48" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K136" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="137" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J137" s="49"/>
+      <c r="J137" s="50"/>
       <c r="K137" s="46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="138" spans="9:18" x14ac:dyDescent="0.3">
@@ -2077,19 +2077,19 @@
     </row>
     <row r="140" spans="9:18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I140" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J140" s="48" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K140" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="141" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J141" s="49"/>
+      <c r="J141" s="50"/>
       <c r="K141" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="142" spans="9:18" x14ac:dyDescent="0.3">
@@ -2097,19 +2097,19 @@
     </row>
     <row r="143" spans="9:18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I143" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J143" s="48" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K143" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="144" spans="9:18" x14ac:dyDescent="0.3">
-      <c r="J144" s="49"/>
+      <c r="J144" s="50"/>
       <c r="K144" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="145" spans="9:11" x14ac:dyDescent="0.3">
@@ -2123,25 +2123,25 @@
     </row>
     <row r="148" spans="9:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I148" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J148" s="48" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K148" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="149" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="J149" s="50"/>
+      <c r="J149" s="49"/>
       <c r="K149" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="150" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="J150" s="49"/>
+      <c r="J150" s="50"/>
       <c r="K150" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="151" spans="9:11" x14ac:dyDescent="0.3">
@@ -2152,39 +2152,39 @@
     </row>
     <row r="153" spans="9:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I153" t="s">
-        <v>191</v>
-      </c>
-      <c r="J153" s="51" t="s">
-        <v>200</v>
+        <v>189</v>
+      </c>
+      <c r="J153" s="53" t="s">
+        <v>198</v>
       </c>
       <c r="K153" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="154" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="J154" s="51"/>
+      <c r="J154" s="53"/>
       <c r="K154" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="155" spans="9:11" x14ac:dyDescent="0.3">
-      <c r="J155" s="51"/>
+      <c r="J155" s="53"/>
       <c r="K155" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J140:J141"/>
+    <mergeCell ref="J143:J144"/>
+    <mergeCell ref="J148:J150"/>
+    <mergeCell ref="J153:J155"/>
+    <mergeCell ref="J136:J137"/>
     <mergeCell ref="J132:J134"/>
     <mergeCell ref="M50:M52"/>
     <mergeCell ref="M55:M58"/>
     <mergeCell ref="M53:M54"/>
     <mergeCell ref="K125:K126"/>
-    <mergeCell ref="J140:J141"/>
-    <mergeCell ref="J143:J144"/>
-    <mergeCell ref="J148:J150"/>
-    <mergeCell ref="J153:J155"/>
-    <mergeCell ref="J136:J137"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2196,7 +2196,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2207,26 +2207,26 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" t="s">
         <v>205</v>
-      </c>
-      <c r="C1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B2">
         <f>(B4*B5)/B6</f>
-        <v>8.3768768251371792</v>
+        <v>102.61674110793045</v>
       </c>
       <c r="C2">
         <f>B2+D2</f>
-        <v>37.376876825137181</v>
+        <v>131.61674110793047</v>
       </c>
       <c r="D2">
         <v>29</v>
@@ -2234,38 +2234,38 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J3" t="s">
+        <v>207</v>
+      </c>
+      <c r="L3" t="s">
+        <v>208</v>
+      </c>
+      <c r="M3" t="s">
         <v>209</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>210</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>211</v>
-      </c>
-      <c r="N3" t="s">
-        <v>212</v>
-      </c>
-      <c r="O3" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B4">
         <f>J4</f>
         <v>1.6200000000000003E-8</v>
       </c>
       <c r="I4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J4">
         <f>1.62 * (10^-8)</f>
         <v>1.6200000000000003E-8</v>
       </c>
       <c r="L4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M4">
         <v>5.1999999999999998E-2</v>
@@ -2281,13 +2281,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B5">
         <v>199</v>
       </c>
       <c r="L5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N5">
         <v>0.9</v>
@@ -2299,14 +2299,14 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B6">
-        <f>PI()*((O6/2)^2)</f>
-        <v>3.8484510006474966E-7</v>
+        <f>PI()*((O7/2)^2)</f>
+        <v>3.1415926535897931E-8</v>
       </c>
       <c r="L6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N6">
         <v>0.7</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N7">
         <v>0.2</v>
@@ -2330,7 +2330,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N8">
         <v>0.1</v>
@@ -2340,22 +2340,30 @@
         <v>1E-4</v>
       </c>
     </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>222</v>
+      </c>
+    </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B11">
         <f>7.9</f>
         <v>7.9</v>
       </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B12">
-        <f>B11/C2</f>
-        <v>0.21136062376102516</v>
+        <f>C11/B2</f>
+        <v>4.8724993076335266E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2573,7 +2581,7 @@
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C37" s="52" t="s">
+      <c r="C37" s="51" t="s">
         <v>5</v>
       </c>
       <c r="E37" s="37" t="s">
@@ -2581,7 +2589,7 @@
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C38" s="52"/>
+      <c r="C38" s="51"/>
       <c r="E38" s="37" t="s">
         <v>137</v>
       </c>
@@ -2621,30 +2629,30 @@
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C52" s="52" t="s">
+      <c r="C52" s="51" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C53" s="52"/>
+      <c r="C53" s="51"/>
       <c r="E53" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C54" s="52"/>
+      <c r="C54" s="51"/>
       <c r="E54" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C55" s="52"/>
+      <c r="C55" s="51"/>
       <c r="E55" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C56" s="52"/>
+      <c r="C56" s="51"/>
       <c r="E56" t="s">
         <v>20</v>
       </c>
@@ -2653,19 +2661,19 @@
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C57" s="52"/>
+      <c r="C57" s="51"/>
       <c r="E57" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C58" s="52"/>
+      <c r="C58" s="51"/>
       <c r="E58" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C59" s="52"/>
+      <c r="C59" s="51"/>
       <c r="E59" t="s">
         <v>13</v>
       </c>
@@ -2674,13 +2682,13 @@
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C60" s="52"/>
+      <c r="C60" s="51"/>
       <c r="E60" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C61" s="52"/>
+      <c r="C61" s="51"/>
       <c r="E61" t="s">
         <v>35</v>
       </c>
@@ -2766,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41353588-76EC-44BD-8AE0-3352EC381993}">
   <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2924,17 +2932,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>113</v>
+        <v>223</v>
       </c>
       <c r="C8" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2">
-        <f>166+169+169</f>
-        <v>504</v>
+        <v>168</v>
       </c>
       <c r="E8" s="54">
-        <f>D8+D9+38</f>
+        <f>(D8*C8)+C9*D9+38</f>
         <v>610</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -3014,28 +3021,13 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="43">
-        <v>10</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" s="43">
-        <v>1</v>
-      </c>
-      <c r="D12" s="27">
-        <v>74</v>
-      </c>
-      <c r="E12" s="27">
-        <f>D12+38</f>
-        <v>112</v>
-      </c>
-      <c r="F12" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>166</v>
-      </c>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
@@ -3043,7 +3035,7 @@
       </c>
       <c r="E19">
         <f>SUM(E3:E13)</f>
-        <v>1930</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -3089,10 +3081,9 @@
     <hyperlink ref="G10" r:id="rId8" xr:uid="{934278AD-0999-4496-8F46-AFBCAE2410AA}"/>
     <hyperlink ref="G11" r:id="rId9" xr:uid="{984CBBDC-41E6-4C5E-9C39-2782D43B70E3}"/>
     <hyperlink ref="G3" r:id="rId10" xr:uid="{A49B1D15-C43A-467C-BE2E-08C1EA8FC185}"/>
-    <hyperlink ref="G12" r:id="rId11" xr:uid="{0424707F-368D-44F3-AAC7-6208FE5A93E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -3323,20 +3314,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="5:16" x14ac:dyDescent="0.3">
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
     </row>
     <row r="2" spans="5:16" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E2" s="2" t="s">

</xml_diff>